<commit_message>
previo para arreglar dashboard
</commit_message>
<xml_diff>
--- a/data/test_data/01_DisenoReactores_Roman_p7r_p32_2casoscienticos.xlsx
+++ b/data/test_data/01_DisenoReactores_Roman_p7r_p32_2casoscienticos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\candidatos_proyectof\tesis_tec\dataReactor\tesis_GUI_sqlite\tesis_pyqt_sqlite\data\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04124D6D-1B1B-40C2-8E53-541E4079EE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D684E99-9F34-401E-B1C6-4408FEA826BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24960" yWindow="17880" windowWidth="18900" windowHeight="11055" xr2:uid="{506660D1-CCA7-4A5E-A616-C57D25E009B2}"/>
+    <workbookView xWindow="-24975" yWindow="19515" windowWidth="21600" windowHeight="11385" xr2:uid="{506660D1-CCA7-4A5E-A616-C57D25E009B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>id</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>0.97571719271322</t>
+  </si>
+  <si>
+    <t>1.056</t>
+  </si>
+  <si>
+    <t>1.137</t>
+  </si>
+  <si>
+    <t>1.219</t>
+  </si>
+  <si>
+    <t>1.249</t>
+  </si>
+  <si>
+    <t>1.279</t>
+  </si>
+  <si>
+    <t>1.336</t>
   </si>
 </sst>
 </file>
@@ -194,7 +212,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +530,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +577,7 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2">
@@ -591,8 +609,8 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1">
-        <v>1056</v>
+      <c r="D3" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -623,8 +641,8 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1">
-        <v>1137</v>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -655,8 +673,8 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1">
-        <v>1219</v>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -687,8 +705,8 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1">
-        <v>1249</v>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -719,8 +737,8 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1">
-        <v>1279</v>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -751,8 +769,8 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1">
-        <v>1336</v>
+      <c r="D8" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>

</xml_diff>